<commit_message>
Added department specific upload for eval templates
changed the eval template controller to add templates to specific
departments listed on the second page of the excel sheet. Changed the
html of the groups page to display the group number instead of group ID.
Changed group controller to not allow the upload of duplicate groups.
</commit_message>
<xml_diff>
--- a/WebBasedEvaluations/Documents/Review_Data_Upload_Users_Company_1.xlsx
+++ b/WebBasedEvaluations/Documents/Review_Data_Upload_Users_Company_1.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\git\Fall-2022-Group-3-Web-Evaluation\WebBasedEvaluations\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD668D4-59BC-45CE-815B-7E6849FC0433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16086FD9-E6ED-4A62-8969-C1BBD0779EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22937C1E-74A3-40E4-BA81-B6A9358BF137}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22937C1E-74A3-40E4-BA81-B6A9358BF137}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="user data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -557,9 +557,6 @@
     <t>Accounting</t>
   </si>
   <si>
-    <t>Saftey</t>
-  </si>
-  <si>
     <t>HR</t>
   </si>
   <si>
@@ -576,6 +573,9 @@
   </si>
   <si>
     <t>DEPT MANAGER</t>
+  </si>
+  <si>
+    <t>Safety</t>
   </si>
 </sst>
 </file>
@@ -971,7 +971,7 @@
   <dimension ref="A1:M83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="J6" sqref="J6:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,10 +1027,10 @@
         <v>148</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>149</v>
@@ -1183,7 +1183,7 @@
         <v>160</v>
       </c>
       <c r="J6" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="K6" t="b">
         <v>0</v>
@@ -1222,7 +1222,7 @@
         <v>160</v>
       </c>
       <c r="J7" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="K7" t="b">
         <v>0</v>
@@ -1261,7 +1261,7 @@
         <v>152</v>
       </c>
       <c r="J8" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="K8" t="b">
         <v>1</v>
@@ -1300,7 +1300,7 @@
         <v>162</v>
       </c>
       <c r="J9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K9" t="b">
         <v>0</v>
@@ -1339,7 +1339,7 @@
         <v>162</v>
       </c>
       <c r="J10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K10" t="b">
         <v>0</v>
@@ -1378,7 +1378,7 @@
         <v>152</v>
       </c>
       <c r="J11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K11" t="b">
         <v>1</v>
@@ -1417,7 +1417,7 @@
         <v>153</v>
       </c>
       <c r="J12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K12" t="b">
         <v>0</v>
@@ -1456,7 +1456,7 @@
         <v>153</v>
       </c>
       <c r="J13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K13" t="b">
         <v>0</v>
@@ -1495,7 +1495,7 @@
         <v>153</v>
       </c>
       <c r="J14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K14" t="b">
         <v>0</v>
@@ -1534,7 +1534,7 @@
         <v>153</v>
       </c>
       <c r="J15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K15" t="b">
         <v>0</v>
@@ -1573,7 +1573,7 @@
         <v>153</v>
       </c>
       <c r="J16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K16" t="b">
         <v>0</v>
@@ -1612,7 +1612,7 @@
         <v>153</v>
       </c>
       <c r="J17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K17" t="b">
         <v>0</v>
@@ -1654,7 +1654,7 @@
         <v>152</v>
       </c>
       <c r="J18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K18" t="b">
         <v>1</v>
@@ -1693,7 +1693,7 @@
         <v>163</v>
       </c>
       <c r="J19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K19" t="b">
         <v>0</v>
@@ -1732,7 +1732,7 @@
         <v>152</v>
       </c>
       <c r="J20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K20" t="b">
         <v>0</v>
@@ -1771,7 +1771,7 @@
         <v>161</v>
       </c>
       <c r="J21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K21" t="b">
         <v>0</v>
@@ -1810,7 +1810,7 @@
         <v>161</v>
       </c>
       <c r="J22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K22" t="b">
         <v>0</v>
@@ -1849,7 +1849,7 @@
         <v>161</v>
       </c>
       <c r="J23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K23" t="b">
         <v>0</v>
@@ -1888,7 +1888,7 @@
         <v>161</v>
       </c>
       <c r="J24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K24" t="b">
         <v>0</v>
@@ -1927,7 +1927,7 @@
         <v>161</v>
       </c>
       <c r="J25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K25" t="b">
         <v>0</v>
@@ -1966,7 +1966,7 @@
         <v>161</v>
       </c>
       <c r="J26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K26" t="b">
         <v>0</v>
@@ -2005,7 +2005,7 @@
         <v>161</v>
       </c>
       <c r="J27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K27" t="b">
         <v>0</v>
@@ -2044,7 +2044,7 @@
         <v>161</v>
       </c>
       <c r="J28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K28" t="b">
         <v>0</v>
@@ -2083,7 +2083,7 @@
         <v>161</v>
       </c>
       <c r="J29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K29" t="b">
         <v>0</v>
@@ -2122,7 +2122,7 @@
         <v>152</v>
       </c>
       <c r="J30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K30" t="b">
         <v>0</v>
@@ -2161,7 +2161,7 @@
         <v>152</v>
       </c>
       <c r="J31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K31" t="b">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>154</v>
       </c>
       <c r="J32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K32" t="b">
         <v>0</v>
@@ -2239,7 +2239,7 @@
         <v>154</v>
       </c>
       <c r="J33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K33" t="b">
         <v>0</v>
@@ -2278,7 +2278,7 @@
         <v>154</v>
       </c>
       <c r="J34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K34" t="b">
         <v>0</v>
@@ -2317,7 +2317,7 @@
         <v>152</v>
       </c>
       <c r="J35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K35" t="b">
         <v>0</v>
@@ -2356,7 +2356,7 @@
         <v>152</v>
       </c>
       <c r="J36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K36" t="b">
         <v>0</v>
@@ -2398,7 +2398,7 @@
         <v>164</v>
       </c>
       <c r="J37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K37" t="b">
         <v>0</v>
@@ -2437,7 +2437,7 @@
         <v>164</v>
       </c>
       <c r="J38" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K38" t="b">
         <v>0</v>
@@ -2476,7 +2476,7 @@
         <v>164</v>
       </c>
       <c r="J39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K39" t="b">
         <v>0</v>
@@ -2515,7 +2515,7 @@
         <v>164</v>
       </c>
       <c r="J40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K40" t="b">
         <v>0</v>
@@ -2554,7 +2554,7 @@
         <v>164</v>
       </c>
       <c r="J41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K41" t="b">
         <v>0</v>
@@ -2593,7 +2593,7 @@
         <v>164</v>
       </c>
       <c r="J42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K42" t="b">
         <v>0</v>
@@ -2632,7 +2632,7 @@
         <v>164</v>
       </c>
       <c r="J43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K43" t="b">
         <v>0</v>
@@ -2671,7 +2671,7 @@
         <v>164</v>
       </c>
       <c r="J44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K44" t="b">
         <v>0</v>
@@ -2710,7 +2710,7 @@
         <v>164</v>
       </c>
       <c r="J45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K45" t="b">
         <v>0</v>
@@ -2983,7 +2983,7 @@
         <v>152</v>
       </c>
       <c r="J52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K52" t="b">
         <v>1</v>
@@ -3022,7 +3022,7 @@
         <v>158</v>
       </c>
       <c r="J53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K53" t="b">
         <v>0</v>
@@ -3061,7 +3061,7 @@
         <v>158</v>
       </c>
       <c r="J54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K54" t="b">
         <v>0</v>
@@ -3100,7 +3100,7 @@
         <v>158</v>
       </c>
       <c r="J55" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K55" t="b">
         <v>0</v>
@@ -3139,7 +3139,7 @@
         <v>158</v>
       </c>
       <c r="J56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K56" t="b">
         <v>0</v>
@@ -3178,7 +3178,7 @@
         <v>158</v>
       </c>
       <c r="J57" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K57" t="b">
         <v>0</v>
@@ -3217,7 +3217,7 @@
         <v>158</v>
       </c>
       <c r="J58" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K58" t="b">
         <v>0</v>
@@ -3256,7 +3256,7 @@
         <v>158</v>
       </c>
       <c r="J59" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K59" t="b">
         <v>0</v>
@@ -3295,7 +3295,7 @@
         <v>158</v>
       </c>
       <c r="J60" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K60" t="b">
         <v>0</v>
@@ -3334,7 +3334,7 @@
         <v>158</v>
       </c>
       <c r="J61" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K61" t="b">
         <v>0</v>
@@ -3373,7 +3373,7 @@
         <v>158</v>
       </c>
       <c r="J62" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K62" t="b">
         <v>0</v>
@@ -3412,7 +3412,7 @@
         <v>158</v>
       </c>
       <c r="J63" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K63" t="b">
         <v>0</v>
@@ -3451,7 +3451,7 @@
         <v>158</v>
       </c>
       <c r="J64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K64" t="b">
         <v>0</v>
@@ -3490,7 +3490,7 @@
         <v>158</v>
       </c>
       <c r="J65" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K65" t="b">
         <v>0</v>
@@ -3529,7 +3529,7 @@
         <v>158</v>
       </c>
       <c r="J66" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K66" t="b">
         <v>0</v>
@@ -3568,7 +3568,7 @@
         <v>152</v>
       </c>
       <c r="J67" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K67" t="b">
         <v>1</v>
@@ -3607,7 +3607,7 @@
         <v>165</v>
       </c>
       <c r="J68" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K68" t="b">
         <v>0</v>
@@ -3646,7 +3646,7 @@
         <v>152</v>
       </c>
       <c r="J69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K69" t="b">
         <v>0</v>
@@ -3685,7 +3685,7 @@
         <v>166</v>
       </c>
       <c r="J70" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K70" t="b">
         <v>0</v>
@@ -3724,7 +3724,7 @@
         <v>152</v>
       </c>
       <c r="J71" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K71" t="b">
         <v>0</v>
@@ -3763,7 +3763,7 @@
         <v>166</v>
       </c>
       <c r="J72" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K72" t="b">
         <v>0</v>
@@ -3802,7 +3802,7 @@
         <v>152</v>
       </c>
       <c r="J73" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K73" t="b">
         <v>0</v>
@@ -3841,7 +3841,7 @@
         <v>156</v>
       </c>
       <c r="J74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K74" t="b">
         <v>0</v>
@@ -3880,7 +3880,7 @@
         <v>156</v>
       </c>
       <c r="J75" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K75" t="b">
         <v>0</v>
@@ -3919,7 +3919,7 @@
         <v>156</v>
       </c>
       <c r="J76" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K76" t="b">
         <v>0</v>
@@ -3958,7 +3958,7 @@
         <v>152</v>
       </c>
       <c r="J77" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K77" t="b">
         <v>0</v>
@@ -3997,7 +3997,7 @@
         <v>152</v>
       </c>
       <c r="J78" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K78" t="b">
         <v>0</v>
@@ -4036,7 +4036,7 @@
         <v>152</v>
       </c>
       <c r="J79" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K79" t="b">
         <v>0</v>
@@ -4075,7 +4075,7 @@
         <v>152</v>
       </c>
       <c r="J80" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K80" t="b">
         <v>0</v>
@@ -4114,7 +4114,7 @@
         <v>152</v>
       </c>
       <c r="J81" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K81" t="b">
         <v>0</v>
@@ -4153,7 +4153,7 @@
         <v>152</v>
       </c>
       <c r="J82" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K82" t="b">
         <v>0</v>
@@ -4192,7 +4192,7 @@
         <v>152</v>
       </c>
       <c r="J83" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K83" t="b">
         <v>0</v>

</xml_diff>